<commit_message>
Added switches to optimization calculation sheet
</commit_message>
<xml_diff>
--- a/calcs/engs125_project.xlsx
+++ b/calcs/engs125_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthverdeflor/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthverdeflor/Documents/EAGLE/projects/audio-amplifier-pcb/calcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE857474-7179-4445-854A-7247DC403A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB0456D-EED0-194C-99A9-377DD409CC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>Part No.</t>
   </si>
@@ -385,9 +385,6 @@
     <t>IRLR3802PBF</t>
   </si>
   <si>
-    <t>Vdd = 6V, Vgs = 25V</t>
-  </si>
-  <si>
     <t>AUIRFZ24NSTRL</t>
   </si>
   <si>
@@ -404,6 +401,18 @@
   </si>
   <si>
     <t>Vdd = 15V, Vgs = 4.5V</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>IRLU3802PBF</t>
+  </si>
+  <si>
+    <t>Vdd = 6V, Vgs = 5V</t>
+  </si>
+  <si>
+    <t>BSZ060NE2LSATMA1</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -756,6 +765,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,14 +1139,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7238D606-EF74-554C-B19A-2497921E86B7}">
-  <dimension ref="B2:H41"/>
+  <dimension ref="A2:H45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="50"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
@@ -1313,7 +1342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
         <v>71</v>
       </c>
@@ -1333,403 +1362,505 @@
         <v>110</v>
       </c>
       <c r="H17" s="49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="C18" s="30">
-        <v>19</v>
+        <v>2.8</v>
       </c>
       <c r="D18" s="30">
         <v>10</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="30">
+        <v>28</v>
+      </c>
+      <c r="F18" s="30">
+        <v>8.5</v>
+      </c>
+      <c r="G18" s="29">
+        <v>110</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="30">
+        <v>19</v>
+      </c>
+      <c r="D19" s="30">
+        <v>10</v>
+      </c>
+      <c r="E19" s="35">
         <v>64</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F19" s="30">
         <v>13.5</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G19" s="29">
         <v>62</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H19" s="33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="14" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="52">
+        <v>3</v>
+      </c>
+      <c r="D20" s="52">
+        <v>2</v>
+      </c>
+      <c r="E20" s="52">
+        <v>8.5</v>
+      </c>
+      <c r="F20" s="52">
+        <v>7.12</v>
+      </c>
+      <c r="G20" s="53">
+        <v>50</v>
+      </c>
+      <c r="H20" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="30">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="52">
+        <v>2.6</v>
+      </c>
+      <c r="D21" s="52">
+        <v>1.7</v>
+      </c>
+      <c r="E21" s="52">
+        <v>7.7</v>
+      </c>
+      <c r="F21" s="52">
+        <v>8.1</v>
+      </c>
+      <c r="G21" s="53">
+        <v>60</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="30">
         <v>3</v>
       </c>
-      <c r="D19" s="30">
-        <v>2</v>
-      </c>
-      <c r="E19" s="30">
-        <v>8.5</v>
-      </c>
-      <c r="F19" s="30">
-        <v>7.12</v>
-      </c>
-      <c r="G19" s="29">
+      <c r="D22" s="30">
+        <v>2.9</v>
+      </c>
+      <c r="E22" s="30">
+        <v>11</v>
+      </c>
+      <c r="F22" s="30">
+        <v>6.4</v>
+      </c>
+      <c r="G22" s="29">
         <v>50</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H22" s="33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="30">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="30">
+        <v>5.3</v>
+      </c>
+      <c r="D23" s="30">
+        <v>7.6</v>
+      </c>
+      <c r="E23" s="30">
+        <v>1.68</v>
+      </c>
+      <c r="F23" s="30">
+        <v>70</v>
+      </c>
+      <c r="G23" s="29">
+        <v>40</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="31">
+        <v>1.6</v>
+      </c>
+      <c r="D24" s="31">
+        <v>3.9</v>
+      </c>
+      <c r="E24" s="31">
+        <v>1</v>
+      </c>
+      <c r="F24" s="31">
+        <v>58</v>
+      </c>
+      <c r="G24" s="32">
+        <v>110</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="30">
-        <v>2.9</v>
-      </c>
-      <c r="E20" s="30">
-        <v>11</v>
-      </c>
-      <c r="F20" s="30">
-        <v>6.4</v>
-      </c>
-      <c r="G20" s="29">
-        <v>50</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="30">
-        <v>5.3</v>
-      </c>
-      <c r="D21" s="30">
-        <v>7.6</v>
-      </c>
-      <c r="E21" s="30">
-        <v>1.68</v>
-      </c>
-      <c r="F21" s="30">
-        <v>70</v>
-      </c>
-      <c r="G21" s="29">
-        <v>40</v>
-      </c>
-      <c r="H21" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="D22" s="31">
-        <v>3.9</v>
-      </c>
-      <c r="E22" s="31">
-        <v>1</v>
-      </c>
-      <c r="F22" s="31">
-        <v>58</v>
-      </c>
-      <c r="G22" s="32">
-        <v>110</v>
-      </c>
-      <c r="H22" s="33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E28" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F28" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
+    <row r="29" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E29" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F29" s="37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="16" t="str">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="16" t="str">
         <f>B14</f>
         <v>IPD220N06L3GBTMA1CT</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C30" s="10">
         <f>(((C14+D14)*$C$3)+(E14*$C$4))*$C$8*10^-9</f>
         <v>0.11950000000000001</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D30" s="10">
         <f>($C$7^2)*F14*10^-3</f>
         <v>2.4750000000000005E-2</v>
       </c>
-      <c r="E28" s="27">
-        <f>SUM(C28:D28)</f>
+      <c r="E30" s="27">
+        <f>SUM(C30:D30)</f>
         <v>0.14425000000000002</v>
       </c>
-      <c r="F28" s="28">
-        <f>E28*G14</f>
+      <c r="F30" s="28">
+        <f>E30*G14</f>
         <v>8.9435000000000002</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="14" t="str">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="str">
         <f>B15</f>
         <v>IPD031N06L3 GCT-ND</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C31" s="10">
         <f>(((C15+D15)*$C$3)+(E15*$C$4))*$C$8*10^-9</f>
         <v>0.61050000000000004</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D31" s="10">
         <f>($C$7^2)*F15*10^-3</f>
         <v>3.4875000000000006E-3</v>
       </c>
-      <c r="E29" s="24">
-        <f t="shared" ref="E29:E36" si="0">SUM(C29:D29)</f>
+      <c r="E31" s="24">
+        <f t="shared" ref="E31:E40" si="0">SUM(C31:D31)</f>
         <v>0.61398750000000002</v>
       </c>
-      <c r="F29" s="11">
-        <f>E29*G15</f>
+      <c r="F31" s="11">
+        <f>E31*G15</f>
         <v>38.067225000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="14" t="str">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="14" t="str">
         <f>B16</f>
         <v>DMN1004UFV-7</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C32" s="10">
         <f>(((C16+D16)*$C$3)+(E16*$C$4))*$C$8*10^-9</f>
         <v>6.9030000000000008E-2</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D32" s="10">
         <f>($C$7^2)*F16*10^-3</f>
         <v>4.2750000000000002E-3</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E32" s="24">
         <f t="shared" si="0"/>
         <v>7.3305000000000009E-2</v>
       </c>
-      <c r="F30" s="11">
-        <f>E30*G16</f>
+      <c r="F32" s="11">
+        <f>E32*G16</f>
         <v>4.8381300000000005</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="14" t="str">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="14" t="str">
         <f>B17</f>
         <v>IRLR3802PBF</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C33" s="10">
         <f>(((C17+D17)*$C$3)+(E17*$C$4))*$C$8*10^-9</f>
         <v>0.2</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D33" s="10">
         <f>($C$7^2)*F17*10^-3</f>
         <v>9.5625000000000016E-3</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E33" s="24">
         <f t="shared" si="0"/>
         <v>0.20956250000000001</v>
       </c>
-      <c r="F31" s="11">
-        <f>E31*G17</f>
+      <c r="F33" s="11">
+        <f>E33*G17</f>
         <v>23.051875000000003</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="14" t="str">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="14" t="str">
         <f>B18</f>
+        <v>IRLU3802PBF</v>
+      </c>
+      <c r="C34" s="10">
+        <f>(((C18+D18)*$C$3)+(E18*$C$4))*$C$8*10^-9</f>
+        <v>0.2</v>
+      </c>
+      <c r="D34" s="10">
+        <f>($C$7^2)*F18*10^-3</f>
+        <v>9.5625000000000016E-3</v>
+      </c>
+      <c r="E34" s="24">
+        <f t="shared" ref="E34" si="1">SUM(C34:D34)</f>
+        <v>0.20956250000000001</v>
+      </c>
+      <c r="F34" s="11">
+        <f>E34*G18</f>
+        <v>23.051875000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="14" t="str">
+        <f>B19</f>
         <v>IPD50N06S4L12ATMACT-ND</v>
       </c>
-      <c r="C32" s="10">
-        <f t="shared" ref="C32" si="1">(((C18+D18)*$C$3)+(E18*$C$4))*$C$8*10^-9</f>
+      <c r="C35" s="10">
+        <f t="shared" ref="C35" si="2">(((C19+D19)*$C$3)+(E19*$C$4))*$C$8*10^-9</f>
         <v>0.45650000000000002</v>
       </c>
-      <c r="D32" s="10">
-        <f>($C$7^2)*F18*10^-3</f>
+      <c r="D35" s="10">
+        <f>($C$7^2)*F19*10^-3</f>
         <v>1.5187500000000003E-2</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E35" s="24">
         <f t="shared" si="0"/>
         <v>0.47168750000000004</v>
       </c>
-      <c r="F32" s="11">
-        <f>E32*G18</f>
+      <c r="F35" s="11">
+        <f>E35*G19</f>
         <v>29.244625000000003</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="14" t="str">
-        <f t="shared" ref="B33:B34" si="2">B19</f>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="51" t="str">
+        <f>B20</f>
         <v>BSC050NE2LSATMA1</v>
       </c>
-      <c r="C33" s="10">
-        <f t="shared" ref="C33:C34" si="3">(((C19+D19)*$C$3)+(E19*$C$4))*$C$8*10^-9</f>
+      <c r="C36" s="54">
+        <f>(((C20+D20)*$C$3)+(E20*$C$4))*$C$8*10^-9</f>
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="D33" s="10">
-        <f t="shared" ref="D33:D34" si="4">($C$7^2)*F19*10^-3</f>
+      <c r="D36" s="54">
+        <f>($C$7^2)*F20*10^-3</f>
         <v>8.0100000000000015E-3</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E36" s="55">
         <f t="shared" si="0"/>
         <v>7.1510000000000004E-2</v>
       </c>
-      <c r="F33" s="11">
-        <f t="shared" ref="F33:F34" si="5">E33*G19</f>
+      <c r="F36" s="56">
+        <f>E36*G20</f>
         <v>3.5755000000000003</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="14" t="str">
-        <f t="shared" si="2"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="51" t="str">
+        <f>B21</f>
+        <v>BSZ060NE2LSATMA1</v>
+      </c>
+      <c r="C37" s="54">
+        <f>(((C21+D21)*$C$3)+(E21*$C$4))*$C$8*10^-9</f>
+        <v>5.6950000000000001E-2</v>
+      </c>
+      <c r="D37" s="54">
+        <f>($C$7^2)*F21*10^-3</f>
+        <v>9.1125000000000008E-3</v>
+      </c>
+      <c r="E37" s="55">
+        <f t="shared" ref="E37" si="3">SUM(C37:D37)</f>
+        <v>6.6062499999999996E-2</v>
+      </c>
+      <c r="F37" s="56">
+        <f>E37*G21</f>
+        <v>3.9637499999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="14" t="str">
+        <f>B22</f>
         <v>BSC0906NS</v>
       </c>
-      <c r="C34" s="10">
-        <f t="shared" si="3"/>
+      <c r="C38" s="10">
+        <f>(((C22+D22)*$C$3)+(E22*$C$4))*$C$8*10^-9</f>
         <v>8.0750000000000002E-2</v>
       </c>
-      <c r="D34" s="10">
-        <f t="shared" si="4"/>
+      <c r="D38" s="10">
+        <f>($C$7^2)*F22*10^-3</f>
         <v>7.2000000000000024E-3</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E38" s="24">
         <f t="shared" si="0"/>
         <v>8.795E-2</v>
       </c>
-      <c r="F34" s="11">
-        <f t="shared" si="5"/>
+      <c r="F38" s="11">
+        <f>E38*G22</f>
         <v>4.3975</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="14" t="str">
-        <f>B21</f>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="14" t="str">
+        <f>B23</f>
         <v>AUIRFZ24NSTRL</v>
       </c>
-      <c r="C35" s="10">
-        <f t="shared" ref="C35" si="6">(((C21+D21)*$C$3)+(E21*$C$4))*$C$8*10^-9</f>
+      <c r="C39" s="10">
+        <f t="shared" ref="C39" si="4">(((C23+D23)*$C$3)+(E23*$C$4))*$C$8*10^-9</f>
         <v>4.233E-2</v>
       </c>
-      <c r="D35" s="10">
-        <f>($C$7^2)*F21*10^-3</f>
+      <c r="D39" s="10">
+        <f>($C$7^2)*F23*10^-3</f>
         <v>7.8750000000000014E-2</v>
       </c>
-      <c r="E35" s="24">
-        <f t="shared" ref="E35" si="7">SUM(C35:D35)</f>
+      <c r="E39" s="24">
+        <f t="shared" ref="E39" si="5">SUM(C39:D39)</f>
         <v>0.12108000000000002</v>
       </c>
-      <c r="F35" s="11">
-        <f t="shared" ref="F35" si="8">E35*G21</f>
+      <c r="F39" s="11">
+        <f t="shared" ref="F39" si="6">E39*G23</f>
         <v>4.8432000000000013</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="str">
-        <f>B22</f>
+    <row r="40" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="15" t="str">
+        <f>B24</f>
         <v>AUIRLR024ZTRLDKR-ND</v>
       </c>
-      <c r="C36" s="12">
-        <f>(((C22+D22)*$C$3)+(E22*$C$4))*$C$8*10^-9</f>
+      <c r="C40" s="12">
+        <f>(((C24+D24)*$C$3)+(E24*$C$4))*$C$8*10^-9</f>
         <v>1.975E-2</v>
       </c>
-      <c r="D36" s="12">
-        <f>($C$7^2)*F22*10^-3</f>
+      <c r="D40" s="12">
+        <f>($C$7^2)*F24*10^-3</f>
         <v>6.5250000000000016E-2</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E40" s="25">
         <f t="shared" si="0"/>
         <v>8.500000000000002E-2</v>
       </c>
-      <c r="F36" s="13">
-        <f>E36*G22</f>
+      <c r="F40" s="13">
+        <f>E40*G24</f>
         <v>9.3500000000000014</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C44" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>11</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C45" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E28:E36">
+  <conditionalFormatting sqref="E30:E40">
     <cfRule type="expression" dxfId="3" priority="7">
-      <formula>E28=MAX($E$28:$E$36)</formula>
+      <formula>E30=MAX($E$30:$E$40)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="8">
-      <formula>E28=MIN($E$28:$E$36)</formula>
+      <formula>E30=MIN($E$30:$E$40)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F36">
+  <conditionalFormatting sqref="F30:F40">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>F28=MAX($F$28:$F$36)</formula>
+      <formula>F30=MAX($F$30:$F$40)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>F28=MIN($F$28:$F$36)</formula>
+      <formula>F30=MIN($F$30:$F$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added efficiency and frequency sweep calculations
</commit_message>
<xml_diff>
--- a/calcs/engs125_project.xlsx
+++ b/calcs/engs125_project.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthverdeflor/Documents/EAGLE/projects/audio-amplifier-pcb/calcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515BB8C0-9602-1544-967E-A1B4BF01D7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3398E577-87B9-3E46-9899-6B29C4191E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches" sheetId="1" r:id="rId1"/>
     <sheet name="Passives" sheetId="8" r:id="rId2"/>
+    <sheet name="Efficiency" sheetId="9" r:id="rId3"/>
+    <sheet name="Frequency" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
   <si>
     <t>Part No.</t>
   </si>
@@ -417,15 +419,156 @@
   <si>
     <t>Quality Factor</t>
   </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Vgg (V)</t>
+  </si>
+  <si>
+    <t>Input Current</t>
+  </si>
+  <si>
+    <t>Gate Drive Current</t>
+  </si>
+  <si>
+    <t>Vin (V)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drain-source swing voltage, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vin</t>
+    </r>
+  </si>
+  <si>
+    <t>Iin (A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Igg (A) </t>
+  </si>
+  <si>
+    <t>Load Resistance</t>
+  </si>
+  <si>
+    <t>Rload (Ω)</t>
+  </si>
+  <si>
+    <t>Efficiency Calculations</t>
+  </si>
+  <si>
+    <t>Output Voltage</t>
+  </si>
+  <si>
+    <t>Output Current</t>
+  </si>
+  <si>
+    <t>Gate Drive Voltage</t>
+  </si>
+  <si>
+    <t>Vout (V)</t>
+  </si>
+  <si>
+    <t>Iout (A)</t>
+  </si>
+  <si>
+    <t>η (%)</t>
+  </si>
+  <si>
+    <t>Input Power</t>
+  </si>
+  <si>
+    <t>Gate Drive Power</t>
+  </si>
+  <si>
+    <t>Output Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin = Vin * Iin </t>
+  </si>
+  <si>
+    <t>Pgg = Vgg * Igg</t>
+  </si>
+  <si>
+    <t>Pout = Vout * Iout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficiency </t>
+  </si>
+  <si>
+    <t>η = Pout / (Pin + Pgg)</t>
+  </si>
+  <si>
+    <t>Switching Frequency</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Load Resistance, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rload</t>
+    </r>
+  </si>
+  <si>
+    <t>fsw (Hz)</t>
+  </si>
+  <si>
+    <t>Magnitude</t>
+  </si>
+  <si>
+    <t>Vref (V)</t>
+  </si>
+  <si>
+    <t>Reference Voltage</t>
+  </si>
+  <si>
+    <t>Frequency Calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnitude </t>
+  </si>
+  <si>
+    <t>|H| (dB)</t>
+  </si>
+  <si>
+    <t>|H|= Vout/Vref</t>
+  </si>
+  <si>
+    <t>Audio Signal</t>
+  </si>
+  <si>
+    <t>measured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measured </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -656,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -788,6 +931,65 @@
     <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,6 +1046,3179 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Converter Efficiency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Load Resistance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Efficiency!$B$14:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Efficiency!$I$14:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>74.91024773854032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.833190765279198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.334466718387347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.423022837608343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.588265539305311</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.848748639825885</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87.268629560350035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.082194470910821</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.753722382324682</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.063126847101358</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.457758085040723</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.218259645523545</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96.278424156354518</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>96.566980481437284</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.037524842483975</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>97.031193192869225</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97.483973774583447</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.910086431200455</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98.133858417365246</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>98.382786925666451</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>98.232671068759586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB9D-D540-BC22-E016ADF6B1CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1186211055"/>
+        <c:axId val="1617068432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1186211055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617068432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1617068432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1186211055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Converter Efficiency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Load Current</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Efficiency!$H$14:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.58899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.73099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.83199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.149</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.421</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.2189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Efficiency!$I$14:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>74.91024773854032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.833190765279198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.334466718387347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.423022837608343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.588265539305311</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.848748639825885</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87.268629560350035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.082194470910821</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.753722382324682</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.063126847101358</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.457758085040723</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.218259645523545</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96.278424156354518</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>96.566980481437284</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.037524842483975</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>97.031193192869225</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97.483973774583447</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.910086431200455</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98.133858417365246</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>98.382786925666451</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>98.232671068759586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A1A8-894E-8DA0-E4E1504ABC51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1186211055"/>
+        <c:axId val="1617068432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1186211055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617068432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1617068432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1186211055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Magnitude </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>vs. Frequency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Frequency!$B$14:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Frequency!$E$14:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>14.848484848484848</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.848484848484848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.803921568627452</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.951456310679612</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.951456310679612</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.140186915887853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.88785046728972</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.009345794392523</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.679245283018869</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.90909090909091</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.410714285714285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.112676056338032</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40.769230769230774</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68.65384615384616</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>84.318181818181827</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>47.303370786516858</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.279069767441861</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.490566037735853</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17.850467289719624</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15.12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.56</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.965517241379311</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.4520547945205475</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.4722222222222232</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.8014184397163131</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.2068965517241388</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-34DC-FF40-A222-7366E40F0E7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1186211055"/>
+        <c:axId val="1617068432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1186211055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617068432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1617068432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1186211055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>146049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>626533</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>33866</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E62DA11-64FC-B04E-AD7D-55FA878EE80D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>728134</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>662517</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>40216</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0888709-6148-7A4C-B6E9-20F7D93DB7BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>146049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>321325</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>198915</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCAE57E9-C6BD-624C-949D-80CE13C740B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1145,8 +4520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7238D606-EF74-554C-B19A-2497921E86B7}">
   <dimension ref="A2:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="107" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView showGridLines="0" topLeftCell="C13" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1875,8 +5250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2283B8F-F30B-5A4A-AF35-A4832B0CC704}">
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="182" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" zoomScale="182" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2067,4 +5442,1457 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020F765E-CAE0-D84D-833F-D8A6B02B0CF5}">
+  <dimension ref="A2:J42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E5" zoomScale="133" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="48"/>
+    <col min="2" max="2" width="27.83203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="8">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="34">
+        <f>SQRT(C6)*C5</f>
+        <v>1.0606601717798214</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9">
+        <v>771000</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="65">
+        <v>60</v>
+      </c>
+      <c r="C14" s="69">
+        <v>12.053000000000001</v>
+      </c>
+      <c r="D14" s="70">
+        <v>0.06</v>
+      </c>
+      <c r="E14" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F14" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G14" s="69">
+        <v>6.1079999999999997</v>
+      </c>
+      <c r="H14" s="70">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I14" s="75">
+        <f>(G14*H14) / (( C14*D14) + (E14*F14)) * 100</f>
+        <v>74.91024773854032</v>
+      </c>
+      <c r="J14" s="33"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="65">
+        <v>55</v>
+      </c>
+      <c r="C15" s="69">
+        <v>12.052</v>
+      </c>
+      <c r="D15" s="70">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E15" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F15" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G15" s="69">
+        <v>6.1710000000000003</v>
+      </c>
+      <c r="H15" s="70">
+        <v>0.108</v>
+      </c>
+      <c r="I15" s="75">
+        <f t="shared" ref="I15:I34" si="0">(G15*H15) / (( C15*D15) + (E15*F15)) * 100</f>
+        <v>76.833190765279198</v>
+      </c>
+      <c r="J15" s="33"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="65">
+        <v>50</v>
+      </c>
+      <c r="C16" s="69">
+        <v>12.051</v>
+      </c>
+      <c r="D16" s="70">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="E16" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F16" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G16" s="69">
+        <v>6.1340000000000003</v>
+      </c>
+      <c r="H16" s="70">
+        <v>0.12</v>
+      </c>
+      <c r="I16" s="75">
+        <f t="shared" si="0"/>
+        <v>78.334466718387347</v>
+      </c>
+      <c r="J16" s="33"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="65">
+        <v>45</v>
+      </c>
+      <c r="C17" s="69">
+        <v>12.05</v>
+      </c>
+      <c r="D17" s="70">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E17" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F17" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G17" s="69">
+        <v>6.15</v>
+      </c>
+      <c r="H17" s="70">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="I17" s="75">
+        <f t="shared" si="0"/>
+        <v>82.423022837608343</v>
+      </c>
+      <c r="J17" s="47"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="65">
+        <v>40</v>
+      </c>
+      <c r="C18" s="69">
+        <v>12.048999999999999</v>
+      </c>
+      <c r="D18" s="70">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E18" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F18" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G18" s="69">
+        <v>6.1680000000000001</v>
+      </c>
+      <c r="H18" s="70">
+        <v>0.15</v>
+      </c>
+      <c r="I18" s="75">
+        <f t="shared" si="0"/>
+        <v>82.588265539305311</v>
+      </c>
+      <c r="J18" s="47"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="65">
+        <v>35</v>
+      </c>
+      <c r="C19" s="69">
+        <v>12.048</v>
+      </c>
+      <c r="D19" s="70">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E19" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F19" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G19" s="69">
+        <v>6.1559999999999997</v>
+      </c>
+      <c r="H19" s="70">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="I19" s="75">
+        <f t="shared" si="0"/>
+        <v>84.848748639825885</v>
+      </c>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="65">
+        <v>30</v>
+      </c>
+      <c r="C20" s="69">
+        <v>12.047000000000001</v>
+      </c>
+      <c r="D20" s="70">
+        <v>0.11</v>
+      </c>
+      <c r="E20" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F20" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G20" s="69">
+        <v>6.149</v>
+      </c>
+      <c r="H20" s="70">
+        <v>0.2</v>
+      </c>
+      <c r="I20" s="75">
+        <f t="shared" si="0"/>
+        <v>87.268629560350035</v>
+      </c>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="65">
+        <v>25</v>
+      </c>
+      <c r="C21" s="69">
+        <v>12.045</v>
+      </c>
+      <c r="D21" s="70">
+        <v>0.13</v>
+      </c>
+      <c r="E21" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F21" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G21" s="69">
+        <v>6.1239999999999997</v>
+      </c>
+      <c r="H21" s="70">
+        <v>0.24</v>
+      </c>
+      <c r="I21" s="75">
+        <f t="shared" si="0"/>
+        <v>89.082194470910821</v>
+      </c>
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="65">
+        <v>20</v>
+      </c>
+      <c r="C22" s="69">
+        <v>12.042</v>
+      </c>
+      <c r="D22" s="70">
+        <v>0.159</v>
+      </c>
+      <c r="E22" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F22" s="70">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G22" s="69">
+        <v>6.1130000000000004</v>
+      </c>
+      <c r="H22" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="I22" s="75">
+        <f t="shared" si="0"/>
+        <v>91.753722382324682</v>
+      </c>
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="65">
+        <v>15</v>
+      </c>
+      <c r="C23" s="69">
+        <v>12.038</v>
+      </c>
+      <c r="D23" s="70">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="E23" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F23" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G23" s="69">
+        <v>6.0890000000000004</v>
+      </c>
+      <c r="H23" s="70">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="I23" s="75">
+        <f t="shared" si="0"/>
+        <v>94.063126847101358</v>
+      </c>
+      <c r="J23" s="33"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="64">
+        <v>10</v>
+      </c>
+      <c r="C24" s="53">
+        <v>12.028</v>
+      </c>
+      <c r="D24" s="68">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="E24" s="52">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F24" s="68">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G24" s="53">
+        <v>6.0330000000000004</v>
+      </c>
+      <c r="H24" s="68">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="I24" s="67">
+        <f t="shared" si="0"/>
+        <v>95.457758085040723</v>
+      </c>
+      <c r="J24" s="33"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="65">
+        <v>9</v>
+      </c>
+      <c r="C25" s="69">
+        <v>12.026</v>
+      </c>
+      <c r="D25" s="70">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="E25" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F25" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G25" s="69">
+        <v>6.0250000000000004</v>
+      </c>
+      <c r="H25" s="70">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="I25" s="75">
+        <f t="shared" si="0"/>
+        <v>96.218259645523545</v>
+      </c>
+      <c r="J25" s="33"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="65">
+        <v>8</v>
+      </c>
+      <c r="C26" s="69">
+        <v>12.022</v>
+      </c>
+      <c r="D26" s="70">
+        <v>0.372</v>
+      </c>
+      <c r="E26" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F26" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G26" s="69">
+        <v>5.9930000000000003</v>
+      </c>
+      <c r="H26" s="70">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="I26" s="75">
+        <f t="shared" si="0"/>
+        <v>96.278424156354518</v>
+      </c>
+      <c r="J26" s="33"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="65">
+        <v>7</v>
+      </c>
+      <c r="C27" s="69">
+        <v>12.016</v>
+      </c>
+      <c r="D27" s="70">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E27" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F27" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G27" s="69">
+        <v>5.976</v>
+      </c>
+      <c r="H27" s="70">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="I27" s="75">
+        <f t="shared" si="0"/>
+        <v>96.566980481437284</v>
+      </c>
+      <c r="J27" s="33"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="65">
+        <v>6</v>
+      </c>
+      <c r="C28" s="69">
+        <v>12.01</v>
+      </c>
+      <c r="D28" s="70">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E28" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F28" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G28" s="69">
+        <v>5.9720000000000004</v>
+      </c>
+      <c r="H28" s="70">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="I28" s="75">
+        <f t="shared" si="0"/>
+        <v>97.037524842483975</v>
+      </c>
+      <c r="J28" s="33"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="65">
+        <v>5</v>
+      </c>
+      <c r="C29" s="69">
+        <v>12.000999999999999</v>
+      </c>
+      <c r="D29" s="70">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E29" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F29" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G29" s="69">
+        <v>5.944</v>
+      </c>
+      <c r="H29" s="70">
+        <v>1.149</v>
+      </c>
+      <c r="I29" s="75">
+        <f t="shared" si="0"/>
+        <v>97.031193192869225</v>
+      </c>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="65">
+        <v>4</v>
+      </c>
+      <c r="C30" s="69">
+        <v>11.989000000000001</v>
+      </c>
+      <c r="D30" s="70">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="E30" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F30" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G30" s="69">
+        <v>5.9260000000000002</v>
+      </c>
+      <c r="H30" s="70">
+        <v>1.421</v>
+      </c>
+      <c r="I30" s="75">
+        <f t="shared" si="0"/>
+        <v>97.483973774583447</v>
+      </c>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="65">
+        <v>3.5</v>
+      </c>
+      <c r="C31" s="69">
+        <v>11.978999999999999</v>
+      </c>
+      <c r="D31" s="70">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="E31" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F31" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G31" s="69">
+        <v>5.9189999999999996</v>
+      </c>
+      <c r="H31" s="70">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="I31" s="75">
+        <f t="shared" si="0"/>
+        <v>97.910086431200455</v>
+      </c>
+      <c r="J31" s="33"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="65">
+        <v>3</v>
+      </c>
+      <c r="C32" s="69">
+        <v>11.967000000000001</v>
+      </c>
+      <c r="D32" s="70">
+        <v>0.93</v>
+      </c>
+      <c r="E32" s="71">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F32" s="70">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G32" s="69">
+        <v>5.8940000000000001</v>
+      </c>
+      <c r="H32" s="70">
+        <v>1.8660000000000001</v>
+      </c>
+      <c r="I32" s="75">
+        <f t="shared" si="0"/>
+        <v>98.133858417365246</v>
+      </c>
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="64">
+        <v>2.5</v>
+      </c>
+      <c r="C33" s="53">
+        <v>11.952999999999999</v>
+      </c>
+      <c r="D33" s="68">
+        <v>1.103</v>
+      </c>
+      <c r="E33" s="52">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F33" s="68">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G33" s="53">
+        <v>5.88</v>
+      </c>
+      <c r="H33" s="68">
+        <v>2.2189999999999999</v>
+      </c>
+      <c r="I33" s="67">
+        <f t="shared" si="0"/>
+        <v>98.382786925666451</v>
+      </c>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="66">
+        <v>2</v>
+      </c>
+      <c r="C34" s="72">
+        <v>11.928000000000001</v>
+      </c>
+      <c r="D34" s="73">
+        <v>1.343</v>
+      </c>
+      <c r="E34" s="74">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="F34" s="73">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G34" s="72">
+        <v>5.835</v>
+      </c>
+      <c r="H34" s="73">
+        <v>2.71</v>
+      </c>
+      <c r="I34" s="76">
+        <f t="shared" si="0"/>
+        <v>98.232671068759586</v>
+      </c>
+      <c r="J34" s="33"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J35" s="33"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I14:I34">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116B25D-0315-C541-8162-FEE8C65F882A}">
+  <dimension ref="A2:F49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="48"/>
+    <col min="2" max="2" width="27.83203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="5" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="8">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="34">
+        <f>SQRT(C6)*C5</f>
+        <v>1.0606601717798214</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="77">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="78">
+        <v>20</v>
+      </c>
+      <c r="C14" s="69">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="D14" s="70">
+        <v>1.47</v>
+      </c>
+      <c r="E14" s="75">
+        <f>D14/C14</f>
+        <v>14.848484848484848</v>
+      </c>
+      <c r="F14" s="33"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="78">
+        <v>100</v>
+      </c>
+      <c r="C15" s="69">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="D15" s="70">
+        <v>1.47</v>
+      </c>
+      <c r="E15" s="75">
+        <f t="shared" ref="E15:E43" si="0">D15/C15</f>
+        <v>14.848484848484848</v>
+      </c>
+      <c r="F15" s="33"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="78">
+        <v>200</v>
+      </c>
+      <c r="C16" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="70">
+        <v>1.49</v>
+      </c>
+      <c r="E16" s="75">
+        <f t="shared" si="0"/>
+        <v>14.899999999999999</v>
+      </c>
+      <c r="F16" s="33"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="78">
+        <v>400</v>
+      </c>
+      <c r="C17" s="69">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="D17" s="70">
+        <v>1.51</v>
+      </c>
+      <c r="E17" s="75">
+        <f t="shared" si="0"/>
+        <v>14.803921568627452</v>
+      </c>
+      <c r="F17" s="47"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="78">
+        <v>800</v>
+      </c>
+      <c r="C18" s="69">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D18" s="70">
+        <v>1.54</v>
+      </c>
+      <c r="E18" s="75">
+        <f t="shared" si="0"/>
+        <v>14.951456310679612</v>
+      </c>
+      <c r="F18" s="47"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="78">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="69">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D19" s="70">
+        <v>1.54</v>
+      </c>
+      <c r="E19" s="75">
+        <f t="shared" si="0"/>
+        <v>14.951456310679612</v>
+      </c>
+      <c r="F19" s="33"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="78">
+        <v>2000</v>
+      </c>
+      <c r="C20" s="69">
+        <v>0.104</v>
+      </c>
+      <c r="D20" s="70">
+        <v>1.56</v>
+      </c>
+      <c r="E20" s="75">
+        <f t="shared" si="0"/>
+        <v>15.000000000000002</v>
+      </c>
+      <c r="F20" s="33"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="78">
+        <v>3000</v>
+      </c>
+      <c r="C21" s="69">
+        <v>0.107</v>
+      </c>
+      <c r="D21" s="70">
+        <v>1.62</v>
+      </c>
+      <c r="E21" s="75">
+        <f t="shared" si="0"/>
+        <v>15.140186915887853</v>
+      </c>
+      <c r="F21" s="33"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="78">
+        <v>4000</v>
+      </c>
+      <c r="C22" s="69">
+        <v>0.107</v>
+      </c>
+      <c r="D22" s="70">
+        <v>1.7</v>
+      </c>
+      <c r="E22" s="75">
+        <f t="shared" si="0"/>
+        <v>15.88785046728972</v>
+      </c>
+      <c r="F22" s="33"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="78">
+        <v>5000</v>
+      </c>
+      <c r="C23" s="69">
+        <v>0.107</v>
+      </c>
+      <c r="D23" s="70">
+        <v>1.82</v>
+      </c>
+      <c r="E23" s="75">
+        <f t="shared" si="0"/>
+        <v>17.009345794392523</v>
+      </c>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="78">
+        <v>6000</v>
+      </c>
+      <c r="C24" s="69">
+        <v>0.106</v>
+      </c>
+      <c r="D24" s="70">
+        <v>1.98</v>
+      </c>
+      <c r="E24" s="75">
+        <f t="shared" si="0"/>
+        <v>18.679245283018869</v>
+      </c>
+      <c r="F24" s="33"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="78">
+        <v>7000</v>
+      </c>
+      <c r="C25" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="D25" s="70">
+        <v>2.19</v>
+      </c>
+      <c r="E25" s="75">
+        <f t="shared" si="0"/>
+        <v>19.90909090909091</v>
+      </c>
+      <c r="F25" s="33"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="78">
+        <v>8000</v>
+      </c>
+      <c r="C26" s="69">
+        <v>0.112</v>
+      </c>
+      <c r="D26" s="70">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E26" s="75">
+        <f t="shared" si="0"/>
+        <v>22.410714285714285</v>
+      </c>
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="78">
+        <v>9000</v>
+      </c>
+      <c r="C27" s="69">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="D27" s="70">
+        <v>1.8</v>
+      </c>
+      <c r="E27" s="75">
+        <f t="shared" si="0"/>
+        <v>25.000000000000004</v>
+      </c>
+      <c r="F27" s="33"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="78">
+        <v>10000</v>
+      </c>
+      <c r="C28" s="69">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D28" s="70">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E28" s="75">
+        <f t="shared" si="0"/>
+        <v>32.112676056338032</v>
+      </c>
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="78">
+        <v>11000</v>
+      </c>
+      <c r="C29" s="69">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D29" s="70">
+        <v>2.12</v>
+      </c>
+      <c r="E29" s="75">
+        <f t="shared" si="0"/>
+        <v>40.769230769230774</v>
+      </c>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="78">
+        <v>12000</v>
+      </c>
+      <c r="C30" s="69">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D30" s="70">
+        <v>3.57</v>
+      </c>
+      <c r="E30" s="75">
+        <f t="shared" si="0"/>
+        <v>68.65384615384616</v>
+      </c>
+      <c r="F30" s="33"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="78">
+        <v>13000</v>
+      </c>
+      <c r="C31" s="69">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D31" s="70">
+        <v>3.71</v>
+      </c>
+      <c r="E31" s="75">
+        <f t="shared" si="0"/>
+        <v>84.318181818181827</v>
+      </c>
+      <c r="F31" s="33"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="78">
+        <v>14000</v>
+      </c>
+      <c r="C32" s="69">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="D32" s="70">
+        <v>4.21</v>
+      </c>
+      <c r="E32" s="75">
+        <f t="shared" si="0"/>
+        <v>47.303370786516858</v>
+      </c>
+      <c r="F32" s="33"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="78">
+        <v>15000</v>
+      </c>
+      <c r="C33" s="69">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D33" s="70">
+        <v>2.69</v>
+      </c>
+      <c r="E33" s="75">
+        <f t="shared" si="0"/>
+        <v>31.279069767441861</v>
+      </c>
+      <c r="F33" s="33"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="78">
+        <v>16000</v>
+      </c>
+      <c r="C34" s="69">
+        <v>0.106</v>
+      </c>
+      <c r="D34" s="70">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E34" s="75">
+        <f t="shared" si="0"/>
+        <v>23.490566037735853</v>
+      </c>
+      <c r="F34" s="33"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="78">
+        <v>17000</v>
+      </c>
+      <c r="C35" s="69">
+        <v>0.107</v>
+      </c>
+      <c r="D35" s="70">
+        <v>1.91</v>
+      </c>
+      <c r="E35" s="75">
+        <f t="shared" si="0"/>
+        <v>17.850467289719624</v>
+      </c>
+      <c r="F35" s="33"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="78">
+        <v>18000</v>
+      </c>
+      <c r="C36" s="69">
+        <v>0.125</v>
+      </c>
+      <c r="D36" s="70">
+        <v>1.89</v>
+      </c>
+      <c r="E36" s="75">
+        <f t="shared" si="0"/>
+        <v>15.12</v>
+      </c>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="78">
+        <v>19000</v>
+      </c>
+      <c r="C37" s="69">
+        <v>0.125</v>
+      </c>
+      <c r="D37" s="70">
+        <v>1.57</v>
+      </c>
+      <c r="E37" s="75">
+        <f t="shared" si="0"/>
+        <v>12.56</v>
+      </c>
+      <c r="F37" s="33"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="78">
+        <v>20000</v>
+      </c>
+      <c r="C38" s="69">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="D38" s="70">
+        <v>1.59</v>
+      </c>
+      <c r="E38" s="75">
+        <f t="shared" si="0"/>
+        <v>10.965517241379311</v>
+      </c>
+      <c r="F38" s="33"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="78">
+        <v>21000</v>
+      </c>
+      <c r="C39" s="69">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D39" s="70">
+        <v>1.38</v>
+      </c>
+      <c r="E39" s="75">
+        <f t="shared" si="0"/>
+        <v>9.4520547945205475</v>
+      </c>
+      <c r="F39" s="33"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="78">
+        <v>22000</v>
+      </c>
+      <c r="C40" s="69">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="D40" s="70">
+        <v>1.22</v>
+      </c>
+      <c r="E40" s="75">
+        <f t="shared" si="0"/>
+        <v>8.4722222222222232</v>
+      </c>
+      <c r="F40" s="33"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="78">
+        <v>23000</v>
+      </c>
+      <c r="C41" s="69">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="D41" s="70">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E41" s="75">
+        <f t="shared" si="0"/>
+        <v>7.8014184397163131</v>
+      </c>
+      <c r="F41" s="33"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="78">
+        <v>24000</v>
+      </c>
+      <c r="C42" s="69">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="D42" s="70">
+        <v>0.98</v>
+      </c>
+      <c r="E42" s="75">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="F42" s="33"/>
+    </row>
+    <row r="43" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="79">
+        <v>25000</v>
+      </c>
+      <c r="C43" s="72">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="D43" s="73">
+        <v>0.9</v>
+      </c>
+      <c r="E43" s="76">
+        <f t="shared" si="0"/>
+        <v>6.2068965517241388</v>
+      </c>
+      <c r="F43" s="33"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="33"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E14:E43">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved frequency sweep magnitude plot
</commit_message>
<xml_diff>
--- a/calcs/engs125_project.xlsx
+++ b/calcs/engs125_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthverdeflor/Documents/EAGLE/projects/audio-amplifier-pcb/calcs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seraph/Documents/EAGLE/projects/audio-amplifier-pcb/calcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3398E577-87B9-3E46-9899-6B29C4191E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5989084E-EA9D-5946-A51B-592A5E50CFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="2" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches" sheetId="1" r:id="rId1"/>
@@ -799,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -990,6 +990,15 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1319,6 +1328,8 @@
         <c:axId val="1186211055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="60"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1336,6 +1347,98 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Load Resistance (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>Ω</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="el-GR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1381,6 +1484,7 @@
         <c:axId val="1617068432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1398,6 +1502,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1779,6 +1938,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Load Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1824,6 +2038,7 @@
         <c:axId val="1617068432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1841,6 +2056,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2145,94 +2415,94 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>14.848484848484848</c:v>
+                  <c:v>23.433642803012521</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.848484848484848</c:v>
+                  <c:v>23.433642803012521</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.899999999999999</c:v>
+                  <c:v>23.46372536824548</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.803921568627452</c:v>
+                  <c:v>23.407535510625038</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.951456310679612</c:v>
+                  <c:v>23.493669922625816</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.951456310679612</c:v>
+                  <c:v>23.493669922625816</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.000000000000002</c:v>
+                  <c:v>23.521825181113627</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.140186915887853</c:v>
+                  <c:v>23.602624737148425</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.88785046728972</c:v>
+                  <c:v>24.021302873861288</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.009345794392523</c:v>
+                  <c:v>24.613752205997304</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.679245283018869</c:v>
+                  <c:v>25.427186499935218</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.90909090909091</c:v>
+                  <c:v>25.981028593637866</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.410714285714285</c:v>
+                  <c:v>27.00911397621713</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.000000000000004</c:v>
+                  <c:v>27.958800173440753</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32.112676056338032</c:v>
+                  <c:v>30.13352996562757</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40.769230769230774</c:v>
+                  <c:v>32.206650345879041</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>68.65384615384616</c:v>
+                  <c:v>36.733297449547884</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>84.318181818181827</c:v>
+                  <c:v>38.518424662577168</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>47.303370786516858</c:v>
+                  <c:v>33.497841783815112</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31.279069767441861</c:v>
+                  <c:v>29.905076575176803</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.490566037735853</c:v>
+                  <c:v>27.417869636619322</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17.850467289719624</c:v>
+                  <c:v>25.03299179125036</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15.12</c:v>
+                  <c:v>23.591035823303752</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.56</c:v>
+                  <c:v>21.979792788023545</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10.965517241379311</c:v>
+                  <c:v>20.800582441709533</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.4520547945205475</c:v>
+                  <c:v>19.510524612335988</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.4722222222222232</c:v>
+                  <c:v>18.559946771589971</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.8014184397163131</c:v>
+                  <c:v>17.843471450056903</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>16.478174818886377</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.2068965517241388</c:v>
+                  <c:v>15.857490144087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2259,6 +2529,7 @@
         <c:axId val="1186211055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="25000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2276,6 +2547,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2321,6 +2651,7 @@
         <c:axId val="1617068432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2338,6 +2669,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Magnitude</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (dB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5448,8 +5838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020F765E-CAE0-D84D-833F-D8A6B02B0CF5}">
   <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E5" zoomScale="133" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6252,8 +6642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116B25D-0315-C541-8162-FEE8C65F882A}">
   <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="88" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6377,9 +6767,9 @@
       <c r="D14" s="70">
         <v>1.47</v>
       </c>
-      <c r="E14" s="75">
-        <f>D14/C14</f>
-        <v>14.848484848484848</v>
+      <c r="E14" s="80">
+        <f>20*LOG10(D14/C14)</f>
+        <v>23.433642803012521</v>
       </c>
       <c r="F14" s="33"/>
     </row>
@@ -6393,9 +6783,9 @@
       <c r="D15" s="70">
         <v>1.47</v>
       </c>
-      <c r="E15" s="75">
-        <f t="shared" ref="E15:E43" si="0">D15/C15</f>
-        <v>14.848484848484848</v>
+      <c r="E15" s="81">
+        <f t="shared" ref="E15:E43" si="0">20*LOG10(D15/C15)</f>
+        <v>23.433642803012521</v>
       </c>
       <c r="F15" s="33"/>
     </row>
@@ -6409,9 +6799,9 @@
       <c r="D16" s="70">
         <v>1.49</v>
       </c>
-      <c r="E16" s="75">
+      <c r="E16" s="81">
         <f t="shared" si="0"/>
-        <v>14.899999999999999</v>
+        <v>23.46372536824548</v>
       </c>
       <c r="F16" s="33"/>
     </row>
@@ -6425,9 +6815,9 @@
       <c r="D17" s="70">
         <v>1.51</v>
       </c>
-      <c r="E17" s="75">
+      <c r="E17" s="81">
         <f t="shared" si="0"/>
-        <v>14.803921568627452</v>
+        <v>23.407535510625038</v>
       </c>
       <c r="F17" s="47"/>
     </row>
@@ -6441,9 +6831,9 @@
       <c r="D18" s="70">
         <v>1.54</v>
       </c>
-      <c r="E18" s="75">
+      <c r="E18" s="81">
         <f t="shared" si="0"/>
-        <v>14.951456310679612</v>
+        <v>23.493669922625816</v>
       </c>
       <c r="F18" s="47"/>
     </row>
@@ -6457,9 +6847,9 @@
       <c r="D19" s="70">
         <v>1.54</v>
       </c>
-      <c r="E19" s="75">
+      <c r="E19" s="81">
         <f t="shared" si="0"/>
-        <v>14.951456310679612</v>
+        <v>23.493669922625816</v>
       </c>
       <c r="F19" s="33"/>
     </row>
@@ -6473,9 +6863,9 @@
       <c r="D20" s="70">
         <v>1.56</v>
       </c>
-      <c r="E20" s="75">
+      <c r="E20" s="81">
         <f t="shared" si="0"/>
-        <v>15.000000000000002</v>
+        <v>23.521825181113627</v>
       </c>
       <c r="F20" s="33"/>
     </row>
@@ -6489,9 +6879,9 @@
       <c r="D21" s="70">
         <v>1.62</v>
       </c>
-      <c r="E21" s="75">
+      <c r="E21" s="81">
         <f t="shared" si="0"/>
-        <v>15.140186915887853</v>
+        <v>23.602624737148425</v>
       </c>
       <c r="F21" s="33"/>
     </row>
@@ -6505,9 +6895,9 @@
       <c r="D22" s="70">
         <v>1.7</v>
       </c>
-      <c r="E22" s="75">
+      <c r="E22" s="81">
         <f t="shared" si="0"/>
-        <v>15.88785046728972</v>
+        <v>24.021302873861288</v>
       </c>
       <c r="F22" s="33"/>
     </row>
@@ -6521,9 +6911,9 @@
       <c r="D23" s="70">
         <v>1.82</v>
       </c>
-      <c r="E23" s="75">
+      <c r="E23" s="81">
         <f t="shared" si="0"/>
-        <v>17.009345794392523</v>
+        <v>24.613752205997304</v>
       </c>
       <c r="F23" s="33"/>
     </row>
@@ -6537,9 +6927,9 @@
       <c r="D24" s="70">
         <v>1.98</v>
       </c>
-      <c r="E24" s="75">
+      <c r="E24" s="81">
         <f t="shared" si="0"/>
-        <v>18.679245283018869</v>
+        <v>25.427186499935218</v>
       </c>
       <c r="F24" s="33"/>
     </row>
@@ -6553,9 +6943,9 @@
       <c r="D25" s="70">
         <v>2.19</v>
       </c>
-      <c r="E25" s="75">
+      <c r="E25" s="81">
         <f t="shared" si="0"/>
-        <v>19.90909090909091</v>
+        <v>25.981028593637866</v>
       </c>
       <c r="F25" s="33"/>
     </row>
@@ -6569,9 +6959,9 @@
       <c r="D26" s="70">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E26" s="75">
+      <c r="E26" s="81">
         <f t="shared" si="0"/>
-        <v>22.410714285714285</v>
+        <v>27.00911397621713</v>
       </c>
       <c r="F26" s="33"/>
     </row>
@@ -6585,9 +6975,9 @@
       <c r="D27" s="70">
         <v>1.8</v>
       </c>
-      <c r="E27" s="75">
+      <c r="E27" s="81">
         <f t="shared" si="0"/>
-        <v>25.000000000000004</v>
+        <v>27.958800173440753</v>
       </c>
       <c r="F27" s="33"/>
     </row>
@@ -6601,9 +6991,9 @@
       <c r="D28" s="70">
         <v>2.2799999999999998</v>
       </c>
-      <c r="E28" s="75">
+      <c r="E28" s="81">
         <f t="shared" si="0"/>
-        <v>32.112676056338032</v>
+        <v>30.13352996562757</v>
       </c>
       <c r="F28" s="33"/>
     </row>
@@ -6617,9 +7007,9 @@
       <c r="D29" s="70">
         <v>2.12</v>
       </c>
-      <c r="E29" s="75">
+      <c r="E29" s="81">
         <f t="shared" si="0"/>
-        <v>40.769230769230774</v>
+        <v>32.206650345879041</v>
       </c>
       <c r="F29" s="33"/>
     </row>
@@ -6633,9 +7023,9 @@
       <c r="D30" s="70">
         <v>3.57</v>
       </c>
-      <c r="E30" s="75">
+      <c r="E30" s="81">
         <f t="shared" si="0"/>
-        <v>68.65384615384616</v>
+        <v>36.733297449547884</v>
       </c>
       <c r="F30" s="33"/>
     </row>
@@ -6649,9 +7039,9 @@
       <c r="D31" s="70">
         <v>3.71</v>
       </c>
-      <c r="E31" s="75">
+      <c r="E31" s="81">
         <f t="shared" si="0"/>
-        <v>84.318181818181827</v>
+        <v>38.518424662577168</v>
       </c>
       <c r="F31" s="33"/>
     </row>
@@ -6665,9 +7055,9 @@
       <c r="D32" s="70">
         <v>4.21</v>
       </c>
-      <c r="E32" s="75">
+      <c r="E32" s="81">
         <f t="shared" si="0"/>
-        <v>47.303370786516858</v>
+        <v>33.497841783815112</v>
       </c>
       <c r="F32" s="33"/>
     </row>
@@ -6681,9 +7071,9 @@
       <c r="D33" s="70">
         <v>2.69</v>
       </c>
-      <c r="E33" s="75">
+      <c r="E33" s="81">
         <f t="shared" si="0"/>
-        <v>31.279069767441861</v>
+        <v>29.905076575176803</v>
       </c>
       <c r="F33" s="33"/>
     </row>
@@ -6697,9 +7087,9 @@
       <c r="D34" s="70">
         <v>2.4900000000000002</v>
       </c>
-      <c r="E34" s="75">
+      <c r="E34" s="81">
         <f t="shared" si="0"/>
-        <v>23.490566037735853</v>
+        <v>27.417869636619322</v>
       </c>
       <c r="F34" s="33"/>
     </row>
@@ -6713,9 +7103,9 @@
       <c r="D35" s="70">
         <v>1.91</v>
       </c>
-      <c r="E35" s="75">
+      <c r="E35" s="81">
         <f t="shared" si="0"/>
-        <v>17.850467289719624</v>
+        <v>25.03299179125036</v>
       </c>
       <c r="F35" s="33"/>
     </row>
@@ -6729,9 +7119,9 @@
       <c r="D36" s="70">
         <v>1.89</v>
       </c>
-      <c r="E36" s="75">
+      <c r="E36" s="81">
         <f t="shared" si="0"/>
-        <v>15.12</v>
+        <v>23.591035823303752</v>
       </c>
       <c r="F36" s="33"/>
     </row>
@@ -6745,9 +7135,9 @@
       <c r="D37" s="70">
         <v>1.57</v>
       </c>
-      <c r="E37" s="75">
+      <c r="E37" s="81">
         <f t="shared" si="0"/>
-        <v>12.56</v>
+        <v>21.979792788023545</v>
       </c>
       <c r="F37" s="33"/>
     </row>
@@ -6761,9 +7151,9 @@
       <c r="D38" s="70">
         <v>1.59</v>
       </c>
-      <c r="E38" s="75">
+      <c r="E38" s="81">
         <f t="shared" si="0"/>
-        <v>10.965517241379311</v>
+        <v>20.800582441709533</v>
       </c>
       <c r="F38" s="33"/>
     </row>
@@ -6777,9 +7167,9 @@
       <c r="D39" s="70">
         <v>1.38</v>
       </c>
-      <c r="E39" s="75">
+      <c r="E39" s="81">
         <f t="shared" si="0"/>
-        <v>9.4520547945205475</v>
+        <v>19.510524612335988</v>
       </c>
       <c r="F39" s="33"/>
     </row>
@@ -6793,9 +7183,9 @@
       <c r="D40" s="70">
         <v>1.22</v>
       </c>
-      <c r="E40" s="75">
+      <c r="E40" s="81">
         <f t="shared" si="0"/>
-        <v>8.4722222222222232</v>
+        <v>18.559946771589971</v>
       </c>
       <c r="F40" s="33"/>
     </row>
@@ -6809,9 +7199,9 @@
       <c r="D41" s="70">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E41" s="75">
+      <c r="E41" s="81">
         <f t="shared" si="0"/>
-        <v>7.8014184397163131</v>
+        <v>17.843471450056903</v>
       </c>
       <c r="F41" s="33"/>
     </row>
@@ -6825,9 +7215,9 @@
       <c r="D42" s="70">
         <v>0.98</v>
       </c>
-      <c r="E42" s="75">
+      <c r="E42" s="81">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
+        <v>16.478174818886377</v>
       </c>
       <c r="F42" s="33"/>
     </row>
@@ -6841,9 +7231,9 @@
       <c r="D43" s="73">
         <v>0.9</v>
       </c>
-      <c r="E43" s="76">
+      <c r="E43" s="82">
         <f t="shared" si="0"/>
-        <v>6.2068965517241388</v>
+        <v>15.857490144087</v>
       </c>
       <c r="F43" s="33"/>
     </row>

</xml_diff>

<commit_message>
Minor revisions to passive components calculation
</commit_message>
<xml_diff>
--- a/calcs/engs125_project.xlsx
+++ b/calcs/engs125_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seraph/Desktop/Dart/W21/ENGS125/PROJECT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthverdeflor/Documents/EAGLE/projects/audio-amplifier-pcb/calcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7678F220-67E8-D144-832C-FFE2F61B884D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42F0FBB-C298-4B4D-BB0C-843311A2BF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="2" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{75B25817-BB02-B742-B7A5-0F6E04A36568}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,6 @@
     <sheet name="Efficiency" sheetId="9" r:id="rId3"/>
     <sheet name="Frequency" sheetId="10" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Frequency!$B$14:$B$43</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Frequency!$F$14:$F$43</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Frequency!$B$14:$B$43</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Frequency!$F$14:$F$43</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Frequency!$B$14:$B$43</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Frequency!$F$14:$F$43</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Frequency!$B$14:$B$43</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Frequency!$F$14:$F$43</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Frequency!$B$14:$B$43</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Frequency!$F$14:$F$43</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="121">
   <si>
     <t>Part No.</t>
   </si>
@@ -242,9 +230,6 @@
   </si>
   <si>
     <t>uC</t>
-  </si>
-  <si>
-    <t>Resistance</t>
   </si>
   <si>
     <t>Ω</t>
@@ -6131,8 +6116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7238D606-EF74-554C-B19A-2497921E86B7}">
   <dimension ref="A2:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6176,7 +6161,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8">
         <v>1.5</v>
@@ -6188,7 +6173,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8">
         <v>0.5</v>
@@ -6311,7 +6296,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="30">
         <v>2.8</v>
@@ -6329,12 +6314,12 @@
         <v>66</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="30">
         <v>2.8</v>
@@ -6352,12 +6337,12 @@
         <v>110</v>
       </c>
       <c r="H17" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="30">
         <v>2.8</v>
@@ -6375,7 +6360,7 @@
         <v>110</v>
       </c>
       <c r="H18" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -6403,10 +6388,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="50">
         <v>3</v>
@@ -6424,15 +6409,15 @@
         <v>50</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="50">
         <v>2.6</v>
@@ -6450,12 +6435,12 @@
         <v>60</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="30">
         <v>3</v>
@@ -6473,12 +6458,12 @@
         <v>50</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="30">
         <v>5.3</v>
@@ -6496,7 +6481,7 @@
         <v>40</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6693,7 +6678,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="49" t="str">
         <f t="shared" si="0"/>
@@ -6718,7 +6703,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="49" t="str">
         <f t="shared" si="0"/>
@@ -6861,8 +6846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2283B8F-F30B-5A4A-AF35-A4832B0CC704}">
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="182" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6880,21 +6865,21 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="46">
         <v>1</v>
@@ -6911,10 +6896,10 @@
         <v>45</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -6931,18 +6916,18 @@
         <v>46</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="41">
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="34">
         <f>C3*SQRT(C5/C4)</f>
@@ -6952,7 +6937,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="38">
         <v>12</v>
@@ -6963,7 +6948,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="8">
         <v>0.5</v>
@@ -6972,23 +6957,23 @@
     </row>
     <row r="9" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="9">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="43">
         <f>C3*SQRT(C5/C4)</f>
@@ -6998,11 +6983,11 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="55">
         <f>C8*(1-C8)*C7 / ((C4*0.000001) * (C9*1000))</f>
-        <v>0.18181818181818185</v>
+        <v>0.12121212121212123</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -7011,11 +6996,11 @@
     </row>
     <row r="15" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="56">
         <f>C14 / (8 * (C5*0.000001) *(C9*1000))</f>
-        <v>3.0303030303030307E-2</v>
+        <v>1.3468013468013469E-2</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -7028,26 +7013,26 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -7059,8 +7044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020F765E-CAE0-D84D-833F-D8A6B02B0CF5}">
   <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="81" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="150" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7092,7 +7077,7 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="8">
         <v>12</v>
@@ -7106,7 +7091,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8">
         <v>1.5</v>
@@ -7120,7 +7105,7 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8">
         <v>0.5</v>
@@ -7155,7 +7140,7 @@
     </row>
     <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -7163,54 +7148,54 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>86</v>
-      </c>
       <c r="G12" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>95</v>
-      </c>
       <c r="I12" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>90</v>
-      </c>
       <c r="G13" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="I13" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
@@ -7811,34 +7796,34 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" t="s">
         <v>106</v>
-      </c>
-      <c r="C42" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -7863,8 +7848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116B25D-0315-C541-8162-FEE8C65F882A}">
   <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="68" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="125" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7894,7 +7879,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="8">
         <v>12</v>
@@ -7905,7 +7890,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8">
         <v>1.5</v>
@@ -7916,7 +7901,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8">
         <v>0.5</v>
@@ -7937,52 +7922,52 @@
     </row>
     <row r="8" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="77">
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F13" s="83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -8015,7 +8000,7 @@
         <v>1.47</v>
       </c>
       <c r="E15" s="81">
-        <f t="shared" ref="E15:F43" si="0">20*LOG10(D15/C15)</f>
+        <f t="shared" ref="E15:E43" si="0">20*LOG10(D15/C15)</f>
         <v>23.433642803012521</v>
       </c>
       <c r="F15" s="75">
@@ -8565,26 +8550,26 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>118</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>